<commit_message>
added provenance to the miflowcyt template
</commit_message>
<xml_diff>
--- a/templates/miflowcyt/MIFlowCyt_template.xlsx
+++ b/templates/miflowcyt/MIFlowCyt_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/ToxRSCat/templates/miflowcyt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{5321E459-2D8B-8C45-AC2D-18ED9EA1F4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94856042-36FF-4BBC-98EC-5D394924F834}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{5321E459-2D8B-8C45-AC2D-18ED9EA1F4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{397B20F2-A81F-414C-A801-B4B6743E17AE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkML_slots" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="211">
   <si>
     <t>description</t>
   </si>
@@ -710,6 +710,9 @@
   </si>
   <si>
     <t>Analysis.wsp</t>
+  </si>
+  <si>
+    <t>provenance</t>
   </si>
 </sst>
 </file>
@@ -762,15 +765,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1105,1455 +1104,1465 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25A47E7-C24D-194E-BA2A-C4B34C2EC6AD}">
-  <dimension ref="A1:R57"/>
+  <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="14.5" style="4" customWidth="1"/>
-    <col min="11" max="12" width="21" style="4" customWidth="1"/>
-    <col min="13" max="13" width="26.875" style="4" customWidth="1"/>
-    <col min="14" max="16" width="21" style="4" customWidth="1"/>
-    <col min="17" max="17" width="34.125" style="4" customWidth="1"/>
-    <col min="18" max="18" width="33" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="11" style="4"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="26.875" customWidth="1"/>
+    <col min="14" max="16" width="21" customWidth="1"/>
+    <col min="17" max="17" width="34.125" customWidth="1"/>
+    <col min="18" max="18" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>154</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>181</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" t="s">
         <v>138</v>
       </c>
-      <c r="O2" s="4" t="b">
+      <c r="O2" t="b">
         <v>1</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" t="s">
         <v>140</v>
       </c>
-      <c r="Q2" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>153</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>155</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
         <v>180</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="4" t="s">
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" t="s">
         <v>139</v>
       </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="4" t="b">
+      <c r="N3" s="1"/>
+      <c r="O3" t="b">
         <v>1</v>
       </c>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="4" t="s">
+      <c r="Q3" s="1"/>
+      <c r="R3" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>156</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" t="s">
         <v>179</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="4" t="s">
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" t="s">
         <v>157</v>
       </c>
-      <c r="O4" s="4" t="b">
+      <c r="O4" t="b">
         <v>1</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>153</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>182</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>178</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="4" t="s">
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" t="s">
         <v>141</v>
       </c>
-      <c r="M5" s="4" t="b">
+      <c r="M5" t="b">
         <v>1</v>
       </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="4" t="b">
+      <c r="N5" s="1"/>
+      <c r="O5" t="b">
         <v>1</v>
       </c>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="4" t="s">
+      <c r="Q5" s="1"/>
+      <c r="R5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L6" s="4" t="s">
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" t="s">
         <v>84</v>
       </c>
-      <c r="N6" s="4" t="b">
+      <c r="N6" t="b">
         <v>1</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="P6" t="s">
         <v>85</v>
       </c>
-      <c r="Q6" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R6" s="4" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R6" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I7" s="4" t="b">
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="4" t="b">
+      <c r="J7" t="b">
         <v>1</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" t="s">
         <v>174</v>
       </c>
-      <c r="N7" s="4" t="b">
+      <c r="N7" t="b">
         <v>1</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" t="s">
         <v>86</v>
       </c>
-      <c r="Q7" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R7" s="4" t="s">
+      <c r="Q7" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R7" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="4" t="b">
+      <c r="I8" t="b">
         <v>1</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" t="s">
         <v>175</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" t="s">
         <v>184</v>
       </c>
-      <c r="O8" s="4" t="b">
+      <c r="O8" t="b">
         <v>1</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" t="s">
         <v>88</v>
       </c>
-      <c r="Q8" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R8" s="4" t="s">
+      <c r="Q8" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R8" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="4" t="b">
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" t="b">
         <v>1</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" t="s">
         <v>186</v>
       </c>
-      <c r="O9" s="4" t="b">
+      <c r="O9" t="b">
         <v>1</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" t="s">
         <v>89</v>
       </c>
-      <c r="Q9" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R9" s="4" t="s">
+      <c r="Q9" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R9" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" t="s">
         <v>108</v>
       </c>
-      <c r="N10" s="4" t="b">
+      <c r="N10" t="b">
         <v>1</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="P10" t="s">
         <v>90</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="Q10" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L11" s="4" t="s">
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" t="s">
         <v>109</v>
       </c>
-      <c r="N11" s="4" t="b">
+      <c r="N11" t="b">
         <v>1</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P11" t="s">
         <v>91</v>
       </c>
-      <c r="Q11" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R11" s="4" t="s">
+      <c r="Q11" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R11" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="4" t="b">
+      <c r="I12" t="b">
         <v>1</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" t="s">
         <v>194</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" t="s">
         <v>110</v>
       </c>
-      <c r="N12" s="4" t="b">
+      <c r="N12" t="b">
         <v>1</v>
       </c>
-      <c r="O12" s="4" t="b">
+      <c r="O12" t="b">
         <v>1</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="P12" t="s">
         <v>92</v>
       </c>
-      <c r="Q12" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R12" s="4" t="s">
+      <c r="Q12" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R12" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s">
         <v>158</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L13" s="4" t="s">
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="L13" t="s">
         <v>162</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="P13" t="s">
         <v>160</v>
       </c>
-      <c r="Q13" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R13" s="4" t="s">
+      <c r="Q13" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R13" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" t="s">
         <v>159</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L14" s="4" t="s">
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" t="s">
         <v>165</v>
       </c>
-      <c r="P14" s="4" t="s">
+      <c r="P14" t="s">
         <v>161</v>
       </c>
-      <c r="Q14" s="5" t="s">
+      <c r="Q14" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" t="s">
         <v>73</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" t="s">
         <v>176</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" t="s">
         <v>111</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="P15" t="s">
         <v>82</v>
       </c>
-      <c r="Q15" s="5" t="s">
+      <c r="Q15" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L16" s="4" t="s">
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+      <c r="L16" t="s">
         <v>112</v>
       </c>
-      <c r="P16" s="4" t="s">
+      <c r="P16" t="s">
         <v>93</v>
       </c>
-      <c r="Q16" s="5" t="s">
+      <c r="Q16" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" t="s">
         <v>73</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" t="s">
         <v>74</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="L17" t="s">
         <v>113</v>
       </c>
-      <c r="P17" s="4" t="s">
+      <c r="P17" t="s">
         <v>94</v>
       </c>
-      <c r="Q17" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R17" s="4" t="s">
+      <c r="Q17" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R17" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" t="s">
         <v>73</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" t="s">
         <v>75</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L18" t="s">
         <v>114</v>
       </c>
-      <c r="P18" s="4" t="s">
+      <c r="P18" t="s">
         <v>95</v>
       </c>
-      <c r="Q18" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R18" s="4" t="s">
+      <c r="Q18" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R18" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" t="s">
         <v>73</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" t="s">
         <v>76</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" t="s">
         <v>115</v>
       </c>
-      <c r="P19" s="4" t="s">
+      <c r="P19" t="s">
         <v>96</v>
       </c>
-      <c r="Q19" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R19" s="4" t="s">
+      <c r="Q19" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R19" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L20" s="4" t="s">
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="L20" t="s">
         <v>116</v>
       </c>
-      <c r="P20" s="4" t="s">
+      <c r="P20" t="s">
         <v>93</v>
       </c>
-      <c r="Q20" s="5" t="s">
+      <c r="Q20" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" t="s">
         <v>73</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" t="s">
         <v>168</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="L21" t="s">
         <v>117</v>
       </c>
-      <c r="P21" s="4" t="s">
+      <c r="P21" t="s">
         <v>83</v>
       </c>
-      <c r="Q21" s="5" t="s">
+      <c r="Q21" s="3" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L22" s="4" t="s">
+      <c r="E22" t="s">
+        <v>72</v>
+      </c>
+      <c r="L22" t="s">
         <v>118</v>
       </c>
-      <c r="P22" s="4" t="s">
+      <c r="P22" t="s">
         <v>97</v>
       </c>
-      <c r="Q22" s="5" t="s">
+      <c r="Q22" s="3" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L23" s="4" t="s">
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="L23" t="s">
         <v>119</v>
       </c>
-      <c r="P23" s="4" t="s">
+      <c r="P23" t="s">
         <v>97</v>
       </c>
-      <c r="Q23" s="5" t="s">
+      <c r="Q23" s="3" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L24" s="4" t="s">
+      <c r="E24" t="s">
+        <v>72</v>
+      </c>
+      <c r="L24" t="s">
         <v>120</v>
       </c>
-      <c r="P24" s="4" t="s">
+      <c r="P24" t="s">
         <v>98</v>
       </c>
-      <c r="Q24" s="5" t="s">
+      <c r="Q24" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="4" t="s">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L25" s="4" t="s">
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+      <c r="L25" t="s">
         <v>121</v>
       </c>
-      <c r="P25" s="4" t="s">
+      <c r="P25" t="s">
         <v>99</v>
       </c>
-      <c r="Q25" s="5" t="s">
+      <c r="Q25" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L26" s="4" t="s">
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+      <c r="L26" t="s">
         <v>122</v>
       </c>
-      <c r="P26" s="4" t="s">
+      <c r="P26" t="s">
         <v>93</v>
       </c>
-      <c r="Q26" s="5" t="s">
+      <c r="Q26" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L27" s="4" t="s">
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+      <c r="L27" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" t="s">
         <v>73</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" t="s">
         <v>177</v>
       </c>
-      <c r="L28" s="4" t="s">
+      <c r="L28" t="s">
         <v>124</v>
       </c>
-      <c r="P28" s="4" t="s">
+      <c r="P28" t="s">
         <v>142</v>
       </c>
-      <c r="Q28" s="5" t="s">
+      <c r="Q28" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" t="s">
         <v>144</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29">
         <v>0</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="L29" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K30" s="4" t="s">
+      <c r="E30" t="s">
+        <v>72</v>
+      </c>
+      <c r="K30" t="s">
         <v>169</v>
       </c>
-      <c r="L30" s="4" t="s">
+      <c r="L30" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" t="s">
         <v>143</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" t="s">
         <v>144</v>
       </c>
-      <c r="L31" s="4" t="s">
+      <c r="L31" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L32" s="4" t="s">
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+      <c r="L32" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="4" t="s">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" t="s">
         <v>73</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="K33" t="s">
         <v>170</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="L33" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="4" t="s">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" t="s">
         <v>62</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L34" s="4" t="s">
+      <c r="E34" t="s">
+        <v>72</v>
+      </c>
+      <c r="L34" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="4" t="s">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" t="s">
         <v>30</v>
       </c>
-      <c r="L35" s="4" t="s">
+      <c r="L35" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="4" t="s">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L36" s="4" t="s">
+      <c r="E36" t="s">
+        <v>72</v>
+      </c>
+      <c r="L36" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" t="s">
         <v>163</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L37" s="4" t="s">
+      <c r="E37" t="s">
+        <v>72</v>
+      </c>
+      <c r="L37" t="s">
         <v>162</v>
       </c>
-      <c r="P37" s="4" t="s">
+      <c r="P37" t="s">
         <v>160</v>
       </c>
-      <c r="Q37" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R37" s="4" t="s">
+      <c r="Q37" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R37" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" s="4" t="s">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" t="s">
         <v>164</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L38" s="4" t="s">
+      <c r="E38" t="s">
+        <v>72</v>
+      </c>
+      <c r="L38" t="s">
         <v>165</v>
       </c>
-      <c r="P38" s="4" t="s">
+      <c r="P38" t="s">
         <v>161</v>
       </c>
-      <c r="Q38" s="5" t="s">
+      <c r="Q38" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="4" t="s">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L39" s="4" t="s">
+      <c r="E39" t="s">
+        <v>72</v>
+      </c>
+      <c r="L39" t="s">
         <v>77</v>
       </c>
-      <c r="N39" s="4" t="b">
+      <c r="N39" t="b">
         <v>1</v>
       </c>
-      <c r="P39" s="4" t="s">
+      <c r="P39" t="s">
         <v>100</v>
       </c>
-      <c r="Q39" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R39" s="4" t="s">
+      <c r="Q39" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R39" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="4" t="s">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L40" s="4" t="s">
+      <c r="E40" t="s">
+        <v>72</v>
+      </c>
+      <c r="L40" t="s">
         <v>130</v>
       </c>
-      <c r="O40" s="4" t="b">
+      <c r="O40" t="b">
         <v>1</v>
       </c>
-      <c r="P40" s="4" t="s">
+      <c r="P40" t="s">
         <v>101</v>
       </c>
-      <c r="Q40" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R40" s="4" t="s">
+      <c r="Q40" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R40" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="4" t="s">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L41" s="4" t="s">
+      <c r="E41" t="s">
+        <v>72</v>
+      </c>
+      <c r="L41" t="s">
         <v>131</v>
       </c>
-      <c r="O41" s="4" t="b">
+      <c r="O41" t="b">
         <v>1</v>
       </c>
-      <c r="P41" s="4" t="s">
+      <c r="P41" t="s">
         <v>102</v>
       </c>
-      <c r="Q41" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R41" s="4" t="s">
+      <c r="Q41" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R41" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="4" t="s">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" t="s">
         <v>39</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L42" s="4" t="s">
+      <c r="E42" t="s">
+        <v>72</v>
+      </c>
+      <c r="L42" t="s">
         <v>132</v>
       </c>
-      <c r="O42" s="4" t="b">
+      <c r="O42" t="b">
         <v>1</v>
       </c>
-      <c r="P42" s="4" t="s">
+      <c r="P42" t="s">
         <v>103</v>
       </c>
-      <c r="Q42" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R42" s="4" t="s">
+      <c r="Q42" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R42" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" s="4" t="s">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L43" s="4" t="s">
+      <c r="E43" t="s">
+        <v>72</v>
+      </c>
+      <c r="L43" t="s">
         <v>133</v>
       </c>
-      <c r="P43" s="4" t="s">
+      <c r="P43" t="s">
         <v>104</v>
       </c>
-      <c r="Q43" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R43" s="4" t="s">
+      <c r="Q43" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R43" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B44" s="4" t="s">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L44" s="4" t="s">
+      <c r="E44" t="s">
+        <v>72</v>
+      </c>
+      <c r="L44" t="s">
         <v>134</v>
       </c>
-      <c r="P44" s="4" t="s">
+      <c r="P44" t="s">
         <v>105</v>
       </c>
-      <c r="Q44" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R44" s="4" t="s">
+      <c r="Q44" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R44" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="4" t="s">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L45" s="4" t="s">
+      <c r="E45" t="s">
+        <v>72</v>
+      </c>
+      <c r="L45" t="s">
         <v>135</v>
       </c>
-      <c r="P45" s="4" t="s">
+      <c r="P45" t="s">
         <v>106</v>
       </c>
-      <c r="Q45" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R45" s="4">
+      <c r="Q45" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R45">
         <v>300607</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="4" t="s">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
         <v>35</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" t="s">
         <v>87</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" t="s">
         <v>73</v>
       </c>
-      <c r="K46" s="4" t="s">
+      <c r="K46" t="s">
         <v>171</v>
       </c>
-      <c r="R46" s="4" t="s">
+      <c r="R46" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" s="4" t="s">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" t="s">
         <v>43</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L47" s="4" t="s">
+      <c r="E47" t="s">
+        <v>72</v>
+      </c>
+      <c r="L47" t="s">
         <v>136</v>
       </c>
-      <c r="P47" s="4" t="s">
+      <c r="P47" t="s">
         <v>93</v>
       </c>
-      <c r="Q47" s="5" t="s">
+      <c r="Q47" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B48" s="4" t="s">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" t="s">
         <v>166</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L48" s="4" t="s">
+      <c r="E48" t="s">
+        <v>72</v>
+      </c>
+      <c r="L48" t="s">
         <v>162</v>
       </c>
-      <c r="P48" s="4" t="s">
+      <c r="P48" t="s">
         <v>160</v>
       </c>
-      <c r="Q48" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R48" s="4" t="s">
+      <c r="Q48" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R48" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" s="4" t="s">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" t="s">
         <v>167</v>
       </c>
-      <c r="E49" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L49" s="4" t="s">
+      <c r="E49" t="s">
+        <v>72</v>
+      </c>
+      <c r="L49" t="s">
         <v>165</v>
       </c>
-      <c r="P49" s="4" t="s">
+      <c r="P49" t="s">
         <v>161</v>
       </c>
-      <c r="Q49" s="5" t="s">
+      <c r="Q49" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50" s="4" t="s">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" t="s">
         <v>24</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L50" s="4" t="s">
+      <c r="E50" t="s">
+        <v>72</v>
+      </c>
+      <c r="L50" t="s">
         <v>137</v>
       </c>
-      <c r="P50" s="4" t="s">
+      <c r="P50" t="s">
         <v>107</v>
       </c>
-      <c r="Q50" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R50" s="4" t="s">
+      <c r="Q50" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R50" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B51" s="4" t="s">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" t="s">
         <v>65</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B52" s="4" t="s">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s">
         <v>23</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L52" s="4" t="s">
+      <c r="E52" t="s">
+        <v>72</v>
+      </c>
+      <c r="L52" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B53" s="4" t="s">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" t="s">
         <v>23</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" t="s">
         <v>67</v>
       </c>
-      <c r="E53" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L53" s="4" t="s">
+      <c r="E53" t="s">
+        <v>72</v>
+      </c>
+      <c r="L53" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" s="4" t="s">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" t="s">
         <v>68</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L54" s="4" t="s">
+      <c r="E54" t="s">
+        <v>72</v>
+      </c>
+      <c r="L54" t="s">
         <v>207</v>
       </c>
-      <c r="R54" s="4" t="s">
+      <c r="R54" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55" s="4" t="s">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L55" s="4" t="s">
+      <c r="E55" t="s">
+        <v>72</v>
+      </c>
+      <c r="L55" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B56" s="4" t="s">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" t="s">
         <v>70</v>
       </c>
-      <c r="E56" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L56" s="4" t="s">
+      <c r="E56" t="s">
+        <v>72</v>
+      </c>
+      <c r="L56" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B57" s="4" t="s">
+      <c r="A57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" t="s">
         <v>23</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" t="s">
         <v>71</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="R57" s="4" t="s">
+      <c r="E57" t="s">
+        <v>72</v>
+      </c>
+      <c r="R57" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" t="s">
+        <v>210</v>
+      </c>
+      <c r="E58" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor revisions to the miflowcyt template and updated some of the documentation including a pdf version
</commit_message>
<xml_diff>
--- a/templates/miflowcyt/MIFlowCyt_template.xlsx
+++ b/templates/miflowcyt/MIFlowCyt_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/ToxRSCat/templates/miflowcyt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/ToxRSCat/templates/miflowcyt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB26455-52F0-1746-B513-7A678106DABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{0BB26455-52F0-1746-B513-7A678106DABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE3FD83A-D4E7-4ADD-9155-2E4CA35FF0A9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkML_slots" sheetId="1" r:id="rId1"/>
@@ -299,9 +299,6 @@
     <t>The instrument has not been altered</t>
   </si>
   <si>
-    <t>The relative amount of molecules, properties, or processes being evaluated (e.g., CD25, apoptosis, membrane permeability, cell viability, oxidative burst). The characteristic(s) being measured shall be provided whenever there is ambiguity about the analyte being measured, such as when sample processing affects detection of the analyte (e.g., propidium iodide example in Table 1). The optical detector (e.g., FL1) or parameter (e.g., FL1-H, see 3.3.6) used primarily for this measurement shall be indicated.</t>
-  </si>
-  <si>
     <t>The purpose of each performed transformation shall be specified (e.g.,
 data visualization, background correction, statistical analysis, quantitative
 flow cytometry, etc.).</t>
@@ -585,13 +582,7 @@
     <t>analysis_protocol_DOI</t>
   </si>
   <si>
-    <t>mercury-vapor lamp; xenon lamp;diode laser; dye laser; gas laser;solid state laser;light-emitting diode;tungsten halogen lamp</t>
-  </si>
-  <si>
     <t>linear;log</t>
-  </si>
-  <si>
-    <t>band pass filter;long pass filter; dichroic long pass filters;short pass filter;dichroic short pass filter; polarizer excitation filter; grating, prism</t>
   </si>
   <si>
     <t>stained;unstained</t>
@@ -716,6 +707,15 @@
   </si>
   <si>
     <t>template version</t>
+  </si>
+  <si>
+    <t>mercury-vapor lamp;xenon lamp;diode laser;dye laser;gas laser;solid state laser;light-emitting diode;tungsten halogen lamp</t>
+  </si>
+  <si>
+    <t>band pass filter;long pass filter;dichroic long pass filters;short pass filter;dichroic short pass filter;polarizer excitation filter;grating, prism</t>
+  </si>
+  <si>
+    <t>The relative amount of molecules, properties, or processes being evaluated (e.g., CD25, apoptosis, membrane permeability, cell viability, oxidative burst). The characteristic(s) being measured shall be provided whenever there is ambiguity about the analyte being measured, such as when sample processing affects detection of the analyte (e.g., propidium iodide example in Table 1). The optical detector (e.g., FL1) or parameter (e.g., FL1-H) used primarily for this measurement shall be indicated.</t>
   </si>
 </sst>
 </file>
@@ -1109,26 +1109,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25A47E7-C24D-194E-BA2A-C4B34C2EC6AD}">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="L29" sqref="A29:L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="46.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.625" customWidth="1"/>
     <col min="5" max="10" width="14.5" customWidth="1"/>
     <col min="11" max="11" width="40.5" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="26.83203125" customWidth="1"/>
+    <col min="13" max="13" width="26.875" customWidth="1"/>
     <col min="14" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="34.1640625" customWidth="1"/>
+    <col min="17" max="17" width="34.125" customWidth="1"/>
     <col min="18" max="18" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1184,50 +1184,50 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
         <v>153</v>
       </c>
-      <c r="C2" t="s">
-        <v>154</v>
-      </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E2" t="s">
         <v>72</v>
       </c>
       <c r="L2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O2" t="b">
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E3" t="s">
         <v>72</v>
@@ -1239,7 +1239,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" t="b">
@@ -1247,21 +1247,21 @@
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E4" t="s">
         <v>72</v>
@@ -1272,27 +1272,27 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O4" t="b">
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E5" t="s">
         <v>72</v>
@@ -1304,7 +1304,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
@@ -1315,10 +1315,10 @@
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1332,22 +1332,22 @@
         <v>72</v>
       </c>
       <c r="L6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N6" t="b">
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1367,22 +1367,22 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="N7" t="b">
         <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1399,25 +1399,25 @@
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="O8" t="b">
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1434,22 +1434,22 @@
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="O9" t="b">
         <v>1</v>
       </c>
       <c r="P9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1463,19 +1463,19 @@
         <v>30</v>
       </c>
       <c r="L10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N10" t="b">
         <v>1</v>
       </c>
       <c r="P10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1489,22 +1489,22 @@
         <v>72</v>
       </c>
       <c r="L11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N11" t="b">
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1521,10 +1521,10 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N12" t="b">
         <v>1</v>
@@ -1533,16 +1533,16 @@
         <v>1</v>
       </c>
       <c r="P12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1550,25 +1550,25 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" t="s">
         <v>72</v>
       </c>
       <c r="L13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R13" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1576,1024 +1576,1024 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" t="s">
+        <v>164</v>
+      </c>
+      <c r="P14" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="L15" t="s">
+        <v>161</v>
+      </c>
+      <c r="P15" t="s">
         <v>159</v>
       </c>
-      <c r="E14" t="s">
-        <v>72</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="Q15" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+      <c r="L16" t="s">
+        <v>164</v>
+      </c>
+      <c r="P16" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="L17" t="s">
+        <v>211</v>
+      </c>
+      <c r="N17" t="b">
+        <v>1</v>
+      </c>
+      <c r="P17" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>72</v>
+      </c>
+      <c r="L18" t="s">
+        <v>129</v>
+      </c>
+      <c r="O18" t="b">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+      <c r="L19" t="s">
+        <v>130</v>
+      </c>
+      <c r="O19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="L20" t="s">
+        <v>131</v>
+      </c>
+      <c r="O20" t="b">
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="L21" t="s">
+        <v>132</v>
+      </c>
+      <c r="P21" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>72</v>
+      </c>
+      <c r="L22" t="s">
+        <v>133</v>
+      </c>
+      <c r="P22" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="L23" t="s">
+        <v>134</v>
+      </c>
+      <c r="P23" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R23">
+        <v>300607</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+      <c r="K24" t="s">
+        <v>168</v>
+      </c>
+      <c r="R24" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+      <c r="L25" t="s">
+        <v>135</v>
+      </c>
+      <c r="P25" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
         <v>165</v>
       </c>
-      <c r="P14" t="s">
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+      <c r="L26" t="s">
         <v>161</v>
       </c>
-      <c r="Q14" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="P26" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R26" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+      <c r="L27" t="s">
+        <v>164</v>
+      </c>
+      <c r="P27" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L28" t="s">
+        <v>136</v>
+      </c>
+      <c r="P28" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" t="s">
+        <v>72</v>
+      </c>
+      <c r="L30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" t="s">
+        <v>72</v>
+      </c>
+      <c r="L31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" t="s">
+        <v>72</v>
+      </c>
+      <c r="L32" t="s">
+        <v>204</v>
+      </c>
+      <c r="R32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" t="s">
+        <v>72</v>
+      </c>
+      <c r="L33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" t="s">
+        <v>72</v>
+      </c>
+      <c r="L34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" t="s">
+        <v>72</v>
+      </c>
+      <c r="R35" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C36" t="s">
         <v>33</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E36" t="s">
         <v>73</v>
       </c>
-      <c r="K15" t="s">
-        <v>176</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="K36" t="s">
+        <v>173</v>
+      </c>
+      <c r="L36" t="s">
+        <v>110</v>
+      </c>
+      <c r="P36" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q36" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" t="s">
+        <v>72</v>
+      </c>
+      <c r="L37" t="s">
         <v>111</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P37" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" t="s">
+        <v>73</v>
+      </c>
+      <c r="K38" t="s">
+        <v>74</v>
+      </c>
+      <c r="L38" t="s">
+        <v>112</v>
+      </c>
+      <c r="P38" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R38" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" t="s">
+        <v>73</v>
+      </c>
+      <c r="K39" t="s">
+        <v>75</v>
+      </c>
+      <c r="L39" t="s">
+        <v>113</v>
+      </c>
+      <c r="P39" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" t="s">
+        <v>73</v>
+      </c>
+      <c r="K40" t="s">
+        <v>76</v>
+      </c>
+      <c r="L40" t="s">
+        <v>114</v>
+      </c>
+      <c r="P40" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="R40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" t="s">
+        <v>72</v>
+      </c>
+      <c r="L41" t="s">
+        <v>115</v>
+      </c>
+      <c r="P41" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" t="s">
+        <v>73</v>
+      </c>
+      <c r="K42" t="s">
+        <v>209</v>
+      </c>
+      <c r="L42" t="s">
+        <v>116</v>
+      </c>
+      <c r="P42" t="s">
         <v>82</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" t="s">
-        <v>72</v>
-      </c>
-      <c r="L16" t="s">
-        <v>112</v>
-      </c>
-      <c r="P16" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" t="s">
-        <v>73</v>
-      </c>
-      <c r="K17" t="s">
-        <v>74</v>
-      </c>
-      <c r="L17" t="s">
-        <v>113</v>
-      </c>
-      <c r="P17" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" t="s">
-        <v>75</v>
-      </c>
-      <c r="L18" t="s">
-        <v>114</v>
-      </c>
-      <c r="P18" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" t="s">
-        <v>73</v>
-      </c>
-      <c r="K19" t="s">
-        <v>76</v>
-      </c>
-      <c r="L19" t="s">
-        <v>115</v>
-      </c>
-      <c r="P19" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" t="s">
-        <v>72</v>
-      </c>
-      <c r="L20" t="s">
-        <v>116</v>
-      </c>
-      <c r="P20" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" t="s">
-        <v>73</v>
-      </c>
-      <c r="K21" t="s">
-        <v>168</v>
-      </c>
-      <c r="L21" t="s">
-        <v>117</v>
-      </c>
-      <c r="P21" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q21" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" t="s">
-        <v>72</v>
-      </c>
-      <c r="L22" t="s">
-        <v>118</v>
-      </c>
-      <c r="P22" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" t="s">
-        <v>72</v>
-      </c>
-      <c r="L23" t="s">
-        <v>119</v>
-      </c>
-      <c r="P23" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" t="s">
-        <v>72</v>
-      </c>
-      <c r="L24" t="s">
-        <v>120</v>
-      </c>
-      <c r="P24" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q24" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" t="s">
-        <v>72</v>
-      </c>
-      <c r="L25" t="s">
-        <v>121</v>
-      </c>
-      <c r="P25" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" t="s">
-        <v>72</v>
-      </c>
-      <c r="L26" t="s">
-        <v>122</v>
-      </c>
-      <c r="P26" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q26" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" t="s">
-        <v>72</v>
-      </c>
-      <c r="L27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" t="s">
-        <v>73</v>
-      </c>
-      <c r="K28" t="s">
-        <v>177</v>
-      </c>
-      <c r="L28" t="s">
-        <v>124</v>
-      </c>
-      <c r="P28" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q28" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" t="s">
-        <v>144</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="L29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" t="s">
-        <v>72</v>
-      </c>
-      <c r="K30" t="s">
-        <v>169</v>
-      </c>
-      <c r="L30" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" t="s">
-        <v>143</v>
-      </c>
-      <c r="E31" t="s">
-        <v>144</v>
-      </c>
-      <c r="L31" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" t="s">
-        <v>72</v>
-      </c>
-      <c r="L32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" t="s">
-        <v>73</v>
-      </c>
-      <c r="K33" t="s">
-        <v>170</v>
-      </c>
-      <c r="L33" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" t="s">
-        <v>62</v>
-      </c>
-      <c r="E34" t="s">
-        <v>72</v>
-      </c>
-      <c r="L34" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" t="s">
-        <v>63</v>
-      </c>
-      <c r="E35" t="s">
-        <v>30</v>
-      </c>
-      <c r="L35" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" t="s">
-        <v>72</v>
-      </c>
-      <c r="L36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" t="s">
-        <v>163</v>
-      </c>
-      <c r="E37" t="s">
-        <v>72</v>
-      </c>
-      <c r="L37" t="s">
-        <v>162</v>
-      </c>
-      <c r="P37" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q37" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R37" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>21</v>
-      </c>
-      <c r="B38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" t="s">
-        <v>164</v>
-      </c>
-      <c r="E38" t="s">
-        <v>72</v>
-      </c>
-      <c r="L38" t="s">
-        <v>165</v>
-      </c>
-      <c r="P38" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q38" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" t="s">
-        <v>72</v>
-      </c>
-      <c r="L39" t="s">
-        <v>77</v>
-      </c>
-      <c r="N39" t="b">
-        <v>1</v>
-      </c>
-      <c r="P39" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q39" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R39" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" t="s">
-        <v>37</v>
-      </c>
-      <c r="E40" t="s">
-        <v>72</v>
-      </c>
-      <c r="L40" t="s">
-        <v>130</v>
-      </c>
-      <c r="O40" t="b">
-        <v>1</v>
-      </c>
-      <c r="P40" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q40" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R40" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" t="s">
-        <v>38</v>
-      </c>
-      <c r="E41" t="s">
-        <v>72</v>
-      </c>
-      <c r="L41" t="s">
-        <v>131</v>
-      </c>
-      <c r="O41" t="b">
-        <v>1</v>
-      </c>
-      <c r="P41" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q41" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R41" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" t="s">
-        <v>39</v>
-      </c>
-      <c r="E42" t="s">
-        <v>72</v>
-      </c>
-      <c r="L42" t="s">
-        <v>132</v>
-      </c>
-      <c r="O42" t="b">
-        <v>1</v>
-      </c>
-      <c r="P42" t="s">
-        <v>103</v>
       </c>
       <c r="Q42" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="R42" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E43" t="s">
         <v>72</v>
       </c>
       <c r="L43" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="P43" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="Q43" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="R43" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E44" t="s">
         <v>72</v>
       </c>
       <c r="L44" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="P44" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="Q44" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="R44" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E45" t="s">
         <v>72</v>
       </c>
       <c r="L45" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="P45" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R45">
-        <v>300607</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="E46" t="s">
+        <v>72</v>
+      </c>
+      <c r="L46" t="s">
+        <v>120</v>
+      </c>
+      <c r="P46" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q46" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" t="s">
+        <v>72</v>
+      </c>
+      <c r="L47" t="s">
+        <v>121</v>
+      </c>
+      <c r="P47" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q47" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s">
+        <v>72</v>
+      </c>
+      <c r="L48" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49" t="s">
         <v>73</v>
       </c>
-      <c r="K46" t="s">
-        <v>171</v>
-      </c>
-      <c r="R46" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" t="s">
-        <v>43</v>
-      </c>
-      <c r="E47" t="s">
-        <v>72</v>
-      </c>
-      <c r="L47" t="s">
-        <v>136</v>
-      </c>
-      <c r="P47" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q47" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>21</v>
-      </c>
-      <c r="B48" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" t="s">
-        <v>166</v>
-      </c>
-      <c r="E48" t="s">
-        <v>72</v>
-      </c>
-      <c r="L48" t="s">
-        <v>162</v>
-      </c>
-      <c r="P48" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q48" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R48" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="K49" t="s">
+        <v>174</v>
+      </c>
+      <c r="L49" t="s">
+        <v>123</v>
+      </c>
+      <c r="P49" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q49" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" t="s">
+        <v>143</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="L50" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" t="s">
+        <v>72</v>
+      </c>
+      <c r="K51" t="s">
         <v>167</v>
       </c>
-      <c r="E49" t="s">
-        <v>72</v>
-      </c>
-      <c r="L49" t="s">
-        <v>165</v>
-      </c>
-      <c r="P49" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q49" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" t="s">
-        <v>72</v>
-      </c>
-      <c r="L50" t="s">
-        <v>137</v>
-      </c>
-      <c r="P50" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q50" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="R50" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>21</v>
-      </c>
-      <c r="B51" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" t="s">
-        <v>65</v>
-      </c>
-      <c r="E51" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="E52" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="L52" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C53" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E53" t="s">
         <v>72</v>
       </c>
       <c r="L53" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C54" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E54" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="K54" t="s">
+        <v>210</v>
       </c>
       <c r="L54" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" t="s">
+        <v>62</v>
+      </c>
+      <c r="E55" t="s">
+        <v>72</v>
+      </c>
+      <c r="L55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E56" t="s">
+        <v>30</v>
+      </c>
+      <c r="L56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" t="s">
+        <v>72</v>
+      </c>
+      <c r="L57" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" t="s">
         <v>207</v>
       </c>
-      <c r="R54" t="s">
+      <c r="C58" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55" t="s">
-        <v>23</v>
-      </c>
-      <c r="C55" t="s">
-        <v>69</v>
-      </c>
-      <c r="E55" t="s">
-        <v>72</v>
-      </c>
-      <c r="L55" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>21</v>
-      </c>
-      <c r="B56" t="s">
-        <v>23</v>
-      </c>
-      <c r="C56" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" t="s">
-        <v>72</v>
-      </c>
-      <c r="L56" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>21</v>
-      </c>
-      <c r="B57" t="s">
-        <v>23</v>
-      </c>
-      <c r="C57" t="s">
-        <v>71</v>
-      </c>
-      <c r="E57" t="s">
-        <v>72</v>
-      </c>
-      <c r="R57" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>21</v>
-      </c>
-      <c r="B58" t="s">
-        <v>210</v>
-      </c>
-      <c r="C58" t="s">
-        <v>211</v>
-      </c>
       <c r="E58" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S1048544">
-    <sortCondition ref="B50:B1048544"/>
+    <sortCondition ref="B58:B1048544"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="Q2" r:id="rId1" xr:uid="{0F9B6DC4-BC59-42C5-AB9C-F44371C8E0BF}"/>
     <hyperlink ref="Q6:Q12" r:id="rId2" display="http://purl.obolibrary.org/obo/" xr:uid="{97CE9ECE-2C1C-4560-A226-AA8CBFA4A2E4}"/>
-    <hyperlink ref="Q15:Q20" r:id="rId3" display="http://purl.obolibrary.org/obo/" xr:uid="{FF3B2C8F-572B-46C6-BEB6-C8AD17CD2D72}"/>
-    <hyperlink ref="Q24:Q26" r:id="rId4" display="http://purl.obolibrary.org/obo/" xr:uid="{08BBAD03-1918-49D4-A5C3-3E0C23518A41}"/>
-    <hyperlink ref="Q28" r:id="rId5" xr:uid="{667234D1-CB21-4DB7-974C-8E7CB4CC67F9}"/>
-    <hyperlink ref="Q21" r:id="rId6" xr:uid="{A1965455-B0C2-4CBB-B6BF-D29546AC50A9}"/>
-    <hyperlink ref="Q22" r:id="rId7" xr:uid="{CB6F9880-AFAB-45F8-BE89-B93BA642CF43}"/>
-    <hyperlink ref="Q23" r:id="rId8" xr:uid="{26DE6419-B906-4973-B77C-64DE00E972B2}"/>
-    <hyperlink ref="Q39:Q45" r:id="rId9" display="http://purl.obolibrary.org/obo/" xr:uid="{CF2DF3FB-DDB3-401F-9F4D-0834276E1F0E}"/>
-    <hyperlink ref="Q47:Q50" r:id="rId10" display="http://purl.obolibrary.org/obo/" xr:uid="{037746AC-447B-4CAB-B897-324FE9B5E48F}"/>
+    <hyperlink ref="Q36:Q41" r:id="rId3" display="http://purl.obolibrary.org/obo/" xr:uid="{FF3B2C8F-572B-46C6-BEB6-C8AD17CD2D72}"/>
+    <hyperlink ref="Q45:Q47" r:id="rId4" display="http://purl.obolibrary.org/obo/" xr:uid="{08BBAD03-1918-49D4-A5C3-3E0C23518A41}"/>
+    <hyperlink ref="Q49" r:id="rId5" xr:uid="{667234D1-CB21-4DB7-974C-8E7CB4CC67F9}"/>
+    <hyperlink ref="Q42" r:id="rId6" xr:uid="{A1965455-B0C2-4CBB-B6BF-D29546AC50A9}"/>
+    <hyperlink ref="Q43" r:id="rId7" xr:uid="{CB6F9880-AFAB-45F8-BE89-B93BA642CF43}"/>
+    <hyperlink ref="Q44" r:id="rId8" xr:uid="{26DE6419-B906-4973-B77C-64DE00E972B2}"/>
+    <hyperlink ref="Q17:Q23" r:id="rId9" display="http://purl.obolibrary.org/obo/" xr:uid="{CF2DF3FB-DDB3-401F-9F4D-0834276E1F0E}"/>
+    <hyperlink ref="Q25:Q28" r:id="rId10" display="http://purl.obolibrary.org/obo/" xr:uid="{037746AC-447B-4CAB-B897-324FE9B5E48F}"/>
     <hyperlink ref="Q13" r:id="rId11" xr:uid="{164C8355-2205-44C3-A9A1-A9CCBB42160E}"/>
     <hyperlink ref="Q14" r:id="rId12" xr:uid="{DAB918FF-8402-43A3-AF4D-54B91B6B4B79}"/>
-    <hyperlink ref="Q37" r:id="rId13" xr:uid="{C5B874AA-3A18-4A66-BA10-134BFC106BC5}"/>
-    <hyperlink ref="Q38" r:id="rId14" xr:uid="{B1549721-C4DE-4F4E-AE15-2B93ABB77392}"/>
-    <hyperlink ref="Q48" r:id="rId15" xr:uid="{35D8B3E8-22E5-4B60-8F71-FC3E42247045}"/>
-    <hyperlink ref="Q49" r:id="rId16" xr:uid="{87229774-19AD-41FE-BD71-50DCE69E8C63}"/>
+    <hyperlink ref="Q15" r:id="rId13" xr:uid="{C5B874AA-3A18-4A66-BA10-134BFC106BC5}"/>
+    <hyperlink ref="Q16" r:id="rId14" xr:uid="{B1549721-C4DE-4F4E-AE15-2B93ABB77392}"/>
+    <hyperlink ref="Q26" r:id="rId15" xr:uid="{35D8B3E8-22E5-4B60-8F71-FC3E42247045}"/>
+    <hyperlink ref="Q27" r:id="rId16" xr:uid="{87229774-19AD-41FE-BD71-50DCE69E8C63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>
@@ -2609,12 +2609,12 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2631,21 +2631,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" t="s">
         <v>148</v>
       </c>
-      <c r="C2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>149</v>
-      </c>
-      <c r="E2" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update export file of miflowcyt
</commit_message>
<xml_diff>
--- a/templates/miflowcyt/MIFlowCyt_template.xlsx
+++ b/templates/miflowcyt/MIFlowCyt_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/ToxRSCat/templates/miflowcyt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB7D9CF-1AC8-5F4F-8188-2CE68956844D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EF9322-1632-2348-A407-EB52B9BA32FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
@@ -1148,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25A47E7-C24D-194E-BA2A-C4B34C2EC6AD}">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="75" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2485,7 +2485,7 @@
         <v>58</v>
       </c>
       <c r="E51" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K51" t="s">
         <v>167</v>

</xml_diff>